<commit_message>
Setting up the Global exception handler in the API
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Шторм\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2922E1C5-B1CD-4A55-8C5E-6E7B0CB5847E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF22648-0D12-F343-A30E-3270D52787F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
     <sheet name="Software" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист1" sheetId="5" r:id="rId3"/>
-    <sheet name="Extensions(Ctrl+Shift+X)" sheetId="3" r:id="rId4"/>
-    <sheet name="DatingApp" sheetId="4" r:id="rId5"/>
+    <sheet name="Extensions(Ctrl+Shift+X)" sheetId="3" r:id="rId3"/>
+    <sheet name="DatingApp" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -195,8 +194,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,7 +479,7 @@
       <selection activeCell="S12" sqref="R12:S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -494,13 +493,13 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -516,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -524,17 +523,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -542,7 +541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -566,32 +565,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE08BD5E-FA49-41BD-9893-2B9501C4A17A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -599,7 +586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -607,57 +594,57 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -668,23 +655,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68EA6-A30D-4F94-98AA-654A95C69E05}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -698,7 +685,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Implement list of users on matches
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Шторм\Desktop\GIT\DatingApp\DatingApp.API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35481D86-828D-4DE6-8EF3-D2FAF291E45F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBB27D2-A168-1F49-A30B-A9F31CDB2B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>https://dotnet.microsoft.com/download</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>AutoMapper.Extensions.Microsoft.DependencyInjection</t>
+  </si>
+  <si>
+    <t>https://www.npmjs.com/package/ngx-gallery</t>
+  </si>
+  <si>
+    <t>npm install ngx-gallery</t>
   </si>
 </sst>
 </file>
@@ -247,8 +253,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,7 +538,7 @@
       <selection activeCell="S12" sqref="R12:S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -540,19 +546,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6168145-A08E-464D-8448-9CCD4F642D06}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -568,7 +574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -576,17 +582,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -594,7 +600,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -602,7 +608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -610,9 +616,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -626,9 +640,10 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{823C37FA-2F81-4C4E-88B5-E2BC733E24CF}"/>
     <hyperlink ref="A9" r:id="rId8" location="/" xr:uid="{A891FF64-EC57-ED43-B75B-FEB6E1F3F62D}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{851C40F4-22DC-BC46-90E1-ACA31D08C680}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{44B05A5B-65EC-8040-8AFD-BD0542FD6857}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -636,17 +651,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -654,7 +669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -662,7 +677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -670,57 +685,57 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -739,18 +754,18 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -773,7 +788,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -796,7 +811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -804,7 +819,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E5" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement cloudinary settings from nuget (v0.13)
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1B044C-E656-4D44-8F18-9CF8D4464EC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE06FE0A-C1DF-DC4B-929E-AD87C5EC2E52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>https://dotnet.microsoft.com/download</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>https://cloudinary.com/</t>
+  </si>
+  <si>
+    <t>CloudinaryDotNet</t>
   </si>
 </sst>
 </file>
@@ -551,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6168145-A08E-464D-8448-9CCD4F642D06}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -660,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -702,6 +705,9 @@
     <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Implement file upload drop method (v0.11-8)
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890766F4-136E-7248-B1A5-4EECCEBA209D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB29B6-D16C-B840-9F28-E7B6DE25BDF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68EA6-A30D-4F94-98AA-654A95C69E05}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="B1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add Publishing to Azure
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EB29B6-D16C-B840-9F28-E7B6DE25BDF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D24647-33D4-F84E-A578-06F2E3FF6F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
     <sheet name="Software" sheetId="2" r:id="rId2"/>
     <sheet name="Extensions(Ctrl+Shift+X)" sheetId="3" r:id="rId3"/>
     <sheet name="DatingApp" sheetId="4" r:id="rId4"/>
+    <sheet name="Собеседование" sheetId="5" r:id="rId5"/>
+    <sheet name="OOP" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>https://dotnet.microsoft.com/download</t>
   </si>
@@ -208,13 +211,88 @@
   </si>
   <si>
     <t>npm install ng2-file-upload --save</t>
+  </si>
+  <si>
+    <t>Что такое кластеризованный и некластеризованный индекс?
+Когда какое надо использовать?</t>
+  </si>
+  <si>
+    <t>http://sql-ex.ru/blogs/optimization/indexes_usage.html</t>
+  </si>
+  <si>
+    <t>Что такое Join? Чем он отличается от Left Join, Right Join? Inner Join? Outer Join?</t>
+  </si>
+  <si>
+    <t>https://shra.ru/2017/09/sql-join-v-primerakh-s-opisaniem/</t>
+  </si>
+  <si>
+    <t>Есть три таблицы:
+CUSTOMERS (ID, NAME, MANAGER_ID);
+MANAGERS (ID, NAME);
+ORDERS (ID, DATE, AMOUNT, CUSTOMER_ID).
+Написать запрос, который выведет имена Customers и их SalesManagers, которые сделали покупок на общую сумму больше 10000 с 01.01.2013.</t>
+  </si>
+  <si>
+    <t>Делаем электронный справочник по книгам. Ищем:
+А) В каком магазине купить данную книгу.
+Б) В каких магазинах купить книги этого автора (авторов).
+В) Кто автор книги.
+Г) Какие книги написал автор.
+Нарисовать БД. Написать запрос Б. (Не забыть учесть, что у одной книжки — может быть несколько авторов)</t>
+  </si>
+  <si>
+    <t>Что такое агрегирующие функции?
+Операторы Group By, Having?
+Приведите примеры их использования.</t>
+  </si>
+  <si>
+    <t>http://dspace.ut.ee/bitstream/handle/10062/10137/_4.html;jsessionid=FC85CA23C239FC2944DE1E3780127E53</t>
+  </si>
+  <si>
+    <t>https://metanit.com/sql/sqlserver/5.2.php</t>
+  </si>
+  <si>
+    <t>Table «PC» (id, cpu(MHz), memory(Mb), hdd(Gb))
+1) Тактовые частоты CPU тех компьютеров, у которых объем памяти 3000 Мб. Вывод: id, cpu, memory.
+2) Минимальный объём жесткого диска, установленного в компьютере на складе. Вывод: hdd.
+3) Количество компьютеров с минимальным объемом жесткого диска, доступного на складе. Вывод: count, hdd.</t>
+  </si>
+  <si>
+    <t>Дана следующая структура базы данных в MS SQL:
+Departments (Id, Name), Employees(Id, DepartmentId, Name, Salary).
+Необходимо:
+• Написать запрос получения имени одного сотрудника, имеющего максимальную зарплату в компании, и название его отдела.
+• Получить список отделов, средняя зарплата в которых больше 1000$.</t>
+  </si>
+  <si>
+    <t>Ado Net – что за технология? и как и когда она используется?</t>
+  </si>
+  <si>
+    <t>https://metanit.com/sharp/adonet/1.1.php</t>
+  </si>
+  <si>
+    <t>Что такое Entity Framework?
+Какие подходы проектирования БД знаете?
+Расскажите про Code First.</t>
+  </si>
+  <si>
+    <t>https://www.internet-technologies.ru/articles/chto-takoe-entity-framework.html</t>
+  </si>
+  <si>
+    <t>https://metanit.com/sharp/entityframework/1.2.php</t>
+  </si>
+  <si>
+    <t>Назовите и объясните основные парадигмы ООП.</t>
+  </si>
+  <si>
+    <t>https://gos-it.fandom.com/wiki/%D0%9E%D1%81%D0%BD%D0%BE%D0%B2%D0%BD%D1%8B%D0%B5_%D0%BF%D1%80%D0%B8%D0%BD%D1%86%D0%B8%D0%BF%D1%8B_%D0%9E%D0%9E%D0%9F:_%D0%B8%D0%BD%D0%BA%D0%B0%D0%BF%D1%81%D1%83%D0%BB%D1%8F%D1%86%D0%B8%D1%8F,_%D0%BD%D0%B0%D1%81%D0%BB%D0%B5%D0%B4%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5,_%D0%BF%D0%BE%D0%BB%D0%B8%D0%BC%D0%BE%D1%80%D1%84%D0%B8%D0%B7%D0%BC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +314,31 @@
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="15"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,13 +362,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -684,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -865,4 +993,142 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F702F2C8-2A2B-9F46-AAE6-419093370E31}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="163.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="122.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="168" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{55687922-2812-AE44-ABEB-C25EF61970D5}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{02E912B4-4F5F-7046-AFF7-752D45083773}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{8D283E40-2C4B-284B-956F-5E814D46091C}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{770E6CD9-552F-8948-8F38-4310A7E6CC6F}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{A3CD5F03-B3EC-0C41-B768-CF7EB05EE0B1}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{89C76AAA-37B1-574A-A612-BE7A22D830C1}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{7EEFDCF7-0694-0A4D-950C-7C083575BEA4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E242CF6-2923-154C-87A1-05F1AC87E708}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="https://gos-it.fandom.com/wiki/%D0%9E%D1%81%D0%BD%D0%BE%D0%B2%D0%BD%D1%8B%D0%B5_%D0%BF%D1%80%D0%B8%D0%BD%D1%86%D0%B8%D0%BF%D1%8B_%D0%9E%D0%9E%D0%9F:_%D0%B8%D0%BD%D0%BA%D0%B0%D0%BF%D1%81%D1%83%D0%BB%D1%8F%D1%86%D0%B8%D1%8F,_%D0%BD%D0%B0%D1%81%D0%BB%D0%B5%D0%B4%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5,_%D0%BF%D0%BE%D0%BB%D0%B8%D0%BC%D0%BE%D1%80%D1%84%D0%B8%D0%B7%D0%BC" xr:uid="{69812A32-D644-2A4A-B9EE-19BA53EA646D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C995D03B-00B0-D446-A59D-1FF1413C42FB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add url to azure
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annaodnostalko/Desktop/GIT/DatingApp/DatingApp.API/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BD7383-7A2D-6541-B8FF-66D09A44D21D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Command" sheetId="1" r:id="rId1"/>
@@ -21,9 +15,9 @@
     <sheet name="OOP" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>https://dotnet.microsoft.com/download</t>
   </si>
@@ -290,12 +284,19 @@
   <si>
     <t>dotnet publish -c Release</t>
   </si>
+  <si>
+    <t>Azure App Service
+ms-azuretools.vscode-azureappservice</t>
+  </si>
+  <si>
+    <t>Set-ExecutionPolicy RemoteSigned -Scope CurrentUser</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +400,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -458,7 +459,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -493,7 +494,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -670,41 +671,41 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S12" sqref="R12:S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6168145-A08E-464D-8448-9CCD4F642D06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,7 +713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -720,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -728,17 +729,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="60">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -746,7 +747,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -754,7 +755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -762,12 +763,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -775,7 +776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -783,7 +784,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -793,18 +794,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{CA4C7DDD-EE3C-4821-B45E-06641689A463}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{F40D6281-7C7A-469C-9EC1-86DF5A3461FE}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{645A4483-8762-4F05-90BC-75FFEBA1414E}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{FC3B0B0D-AFE0-4C7E-AEBC-23A7F6F260CC}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{9E934F90-6341-408D-8981-4C6560FBBF52}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{02D5A21E-88F4-4A97-B73C-1AAB884B7647}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{823C37FA-2F81-4C4E-88B5-E2BC733E24CF}"/>
-    <hyperlink ref="A9" r:id="rId8" location="/" xr:uid="{A891FF64-EC57-ED43-B75B-FEB6E1F3F62D}"/>
-    <hyperlink ref="A10" r:id="rId9" xr:uid="{851C40F4-22DC-BC46-90E1-ACA31D08C680}"/>
-    <hyperlink ref="A11" r:id="rId10" xr:uid="{44B05A5B-65EC-8040-8AFD-BD0542FD6857}"/>
-    <hyperlink ref="A12" r:id="rId11" xr:uid="{18CEA049-AFD0-4B46-8859-2CC00DAD55AC}"/>
-    <hyperlink ref="A13" r:id="rId12" xr:uid="{EA66C20C-92F1-D549-A17A-FB141628B5CC}"/>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8" location="/"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
@@ -812,20 +813,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB87434-8813-4BA3-A177-924FB2B1AB09}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -833,7 +834,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="30">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -841,7 +842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -849,12 +850,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="B4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="30">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -862,49 +863,54 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="30">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="30">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="30">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="30">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="30">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30">
+      <c r="A15" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -914,26 +920,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F68EA6-A30D-4F94-98AA-654A95C69E05}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="162" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.83203125" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -956,7 +963,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -984,8 +991,11 @@
       <c r="K2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -993,7 +1003,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="E5" s="3"/>
     </row>
   </sheetData>
@@ -1003,21 +1013,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F702F2C8-2A2B-9F46-AAE6-419093370E31}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="163.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="122.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="163.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="122.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="46.5">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1026,7 +1036,7 @@
       </c>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:4" ht="23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="23.25">
       <c r="A2" s="10" t="s">
         <v>56</v>
       </c>
@@ -1035,17 +1045,17 @@
       </c>
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="139.5">
       <c r="A3" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="162.75">
       <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="60.75">
       <c r="A5" s="11" t="s">
         <v>60</v>
       </c>
@@ -1056,17 +1066,17 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="139.5">
       <c r="A6" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="168" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="162.75">
       <c r="A7" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="20.25">
       <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
@@ -1074,7 +1084,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="60.75">
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
@@ -1087,32 +1097,32 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{55687922-2812-AE44-ABEB-C25EF61970D5}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{02E912B4-4F5F-7046-AFF7-752D45083773}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{8D283E40-2C4B-284B-956F-5E814D46091C}"/>
-    <hyperlink ref="B8" r:id="rId4" xr:uid="{770E6CD9-552F-8948-8F38-4310A7E6CC6F}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{A3CD5F03-B3EC-0C41-B768-CF7EB05EE0B1}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{89C76AAA-37B1-574A-A612-BE7A22D830C1}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{7EEFDCF7-0694-0A4D-950C-7C083575BEA4}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E242CF6-2923-154C-87A1-05F1AC87E708}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="20.25">
       <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
@@ -1122,19 +1132,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://gos-it.fandom.com/wiki/%D0%9E%D1%81%D0%BD%D0%BE%D0%B2%D0%BD%D1%8B%D0%B5_%D0%BF%D1%80%D0%B8%D0%BD%D1%86%D0%B8%D0%BF%D1%8B_%D0%9E%D0%9E%D0%9F:_%D0%B8%D0%BD%D0%BA%D0%B0%D0%BF%D1%81%D1%83%D0%BB%D1%8F%D1%86%D0%B8%D1%8F,_%D0%BD%D0%B0%D1%81%D0%BB%D0%B5%D0%B4%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5,_%D0%BF%D0%BE%D0%BB%D0%B8%D0%BC%D0%BE%D1%80%D1%84%D0%B8%D0%B7%D0%BC" xr:uid="{69812A32-D644-2A4A-B9EE-19BA53EA646D}"/>
+    <hyperlink ref="B1" r:id="rId1" display="https://gos-it.fandom.com/wiki/%D0%9E%D1%81%D0%BD%D0%BE%D0%B2%D0%BD%D1%8B%D0%B5_%D0%BF%D1%80%D0%B8%D0%BD%D1%86%D0%B8%D0%BF%D1%8B_%D0%9E%D0%9E%D0%9F:_%D0%B8%D0%BD%D0%BA%D0%B0%D0%BF%D1%81%D1%83%D0%BB%D1%8F%D1%86%D0%B8%D1%8F,_%D0%BD%D0%B0%D1%81%D0%BB%D0%B5%D0%B4%D0%BE%D0%B2%D0%B0%D0%BD%D0%B8%D0%B5,_%D0%BF%D0%BE%D0%BB%D0%B8%D0%BC%D0%BE%D1%80%D1%84%D0%B8%D0%B7%D0%BC"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C995D03B-00B0-D446-A59D-1FF1413C42FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>